<commit_message>
removing form no longer needed, making `patient_id` mandatory in all forms, adding role to the nurse-create form
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_visit.xlsx
+++ b/config/itech-aurum/forms/app/client_visit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-67\itech-aurum\forms\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-78\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3A7712-2110-4ED2-B7BB-256CBE29F449}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F15310-743E-45DF-9067-8247F2B2A98A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15825" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="112">
   <si>
     <t>type</t>
   </si>
@@ -930,10 +930,10 @@
   <dimension ref="A1:K23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1088,7 +1088,9 @@
       <c r="E6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>40</v>
+      </c>
       <c r="G6" s="17"/>
       <c r="H6" s="17"/>
       <c r="I6" s="17" t="s">

</xml_diff>

<commit_message>
Making client_visit available in the reports tab, hiding some contact fields
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_visit.xlsx
+++ b/config/itech-aurum/forms/app/client_visit.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-78\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60F15310-743E-45DF-9067-8247F2B2A98A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A3735B-BAFF-457D-9B91-F162F53F4C56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -933,7 +933,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1101,7 +1101,7 @@
     </row>
     <row r="7" spans="1:11">
       <c r="A7" s="11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B7" s="11" t="s">
         <v>1</v>
@@ -1120,7 +1120,7 @@
     </row>
     <row r="8" spans="1:11">
       <c r="A8" s="11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="B8" s="11" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
Hiding fields not required to be seen in the reports tab, Change constraints in enroll form Updates tests for the enroll form changes
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_visit.xlsx
+++ b/config/itech-aurum/forms/app/client_visit.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-78\itech-aurum\forms\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-81\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15A3735B-BAFF-457D-9B91-F162F53F4C56}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2E6658-09D7-4BD3-A374-5B1617A1744B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="113">
   <si>
     <t>type</t>
   </si>
@@ -363,6 +363,9 @@
   </si>
   <si>
     <t>regex(., '^(AN|BL|IN|OT|PA|SD|SX|WD|OA)-[A-C]$')</t>
+  </si>
+  <si>
+    <t>instance::tag</t>
   </si>
 </sst>
 </file>
@@ -927,13 +930,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K23"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -949,11 +952,12 @@
     <col min="9" max="9" width="27.375" style="20" customWidth="1"/>
     <col min="10" max="10" width="12.5" style="7"/>
     <col min="11" max="11" width="20.625" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="1025" width="12.5" style="7"/>
+    <col min="12" max="12" width="13.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="13" max="1025" width="12.5" style="7"/>
     <col min="1026" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="6" customFormat="1" ht="15.75">
+    <row r="1" spans="1:12" s="6" customFormat="1" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -987,8 +991,11 @@
       <c r="K1" s="15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11">
+      <c r="L1" s="6" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" s="11" t="s">
         <v>11</v>
       </c>
@@ -1010,8 +1017,9 @@
       <c r="I2" s="16"/>
       <c r="J2" s="11"/>
       <c r="K2" s="16"/>
-    </row>
-    <row r="3" spans="1:11">
+      <c r="L2" s="16"/>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
@@ -1033,8 +1041,9 @@
         <v>19</v>
       </c>
       <c r="K3" s="17"/>
-    </row>
-    <row r="4" spans="1:11">
+      <c r="L3" s="17"/>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" s="11" t="s">
         <v>15</v>
       </c>
@@ -1054,8 +1063,9 @@
       <c r="I4" s="17"/>
       <c r="J4" s="10"/>
       <c r="K4" s="17"/>
-    </row>
-    <row r="5" spans="1:11">
+      <c r="L4" s="17"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
@@ -1073,8 +1083,9 @@
       <c r="I5" s="17"/>
       <c r="J5" s="10"/>
       <c r="K5" s="17"/>
-    </row>
-    <row r="6" spans="1:11">
+      <c r="L5" s="17"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
@@ -1098,8 +1109,9 @@
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="17"/>
-    </row>
-    <row r="7" spans="1:11">
+      <c r="L6" s="17"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" s="11" t="s">
         <v>18</v>
       </c>
@@ -1117,8 +1129,9 @@
       <c r="I7" s="17"/>
       <c r="J7" s="10"/>
       <c r="K7" s="17"/>
-    </row>
-    <row r="8" spans="1:11">
+      <c r="L7" s="17"/>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
@@ -1136,8 +1149,9 @@
       <c r="I8" s="17"/>
       <c r="J8" s="10"/>
       <c r="K8" s="17"/>
-    </row>
-    <row r="9" spans="1:11">
+      <c r="L8" s="17"/>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
@@ -1151,8 +1165,9 @@
       <c r="I9" s="17"/>
       <c r="J9" s="10"/>
       <c r="K9" s="17"/>
-    </row>
-    <row r="10" spans="1:11">
+      <c r="L9" s="17"/>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" s="11" t="s">
         <v>32</v>
       </c>
@@ -1166,8 +1181,12 @@
       <c r="I10" s="16"/>
       <c r="J10" s="11"/>
       <c r="K10" s="16"/>
-    </row>
-    <row r="12" spans="1:11">
+      <c r="L10" s="16"/>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="L11" s="20"/>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" s="13" t="s">
         <v>33</v>
       </c>
@@ -1187,8 +1206,9 @@
       <c r="K12" s="18" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="13" spans="1:11">
+      <c r="L12" s="18"/>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" s="13" t="s">
         <v>33</v>
       </c>
@@ -1208,8 +1228,9 @@
       <c r="K13" s="18" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="14" spans="1:11">
+      <c r="L13" s="18"/>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" s="13" t="s">
         <v>33</v>
       </c>
@@ -1231,8 +1252,11 @@
       <c r="K14" s="18" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="105">
+      <c r="L14" s="18" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="105">
       <c r="A15" s="14" t="s">
         <v>42</v>
       </c>
@@ -1250,8 +1274,9 @@
       <c r="I15" s="19"/>
       <c r="J15" s="14"/>
       <c r="K15" s="19"/>
-    </row>
-    <row r="16" spans="1:11">
+      <c r="L15" s="19"/>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -1271,8 +1296,9 @@
       <c r="I16" s="19"/>
       <c r="J16" s="14"/>
       <c r="K16" s="19"/>
-    </row>
-    <row r="17" spans="1:11">
+      <c r="L16" s="19"/>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17" s="14" t="s">
         <v>48</v>
       </c>
@@ -1294,8 +1320,9 @@
       <c r="I17" s="19"/>
       <c r="J17" s="14"/>
       <c r="K17" s="19"/>
-    </row>
-    <row r="18" spans="1:11">
+      <c r="L17" s="19"/>
+    </row>
+    <row r="18" spans="1:12">
       <c r="A18" s="14" t="s">
         <v>15</v>
       </c>
@@ -1317,8 +1344,9 @@
       <c r="I18" s="19"/>
       <c r="J18" s="14"/>
       <c r="K18" s="19"/>
-    </row>
-    <row r="19" spans="1:11" ht="25.5">
+      <c r="L18" s="19"/>
+    </row>
+    <row r="19" spans="1:12" ht="25.5">
       <c r="A19" s="14" t="s">
         <v>52</v>
       </c>
@@ -1344,8 +1372,9 @@
         <v>56</v>
       </c>
       <c r="K19" s="19"/>
-    </row>
-    <row r="20" spans="1:11">
+      <c r="L19" s="19"/>
+    </row>
+    <row r="20" spans="1:12">
       <c r="A20" s="14" t="s">
         <v>57</v>
       </c>
@@ -1365,8 +1394,9 @@
       <c r="I20" s="19"/>
       <c r="J20" s="14"/>
       <c r="K20" s="19"/>
-    </row>
-    <row r="21" spans="1:11" ht="60">
+      <c r="L20" s="19"/>
+    </row>
+    <row r="21" spans="1:12" ht="60">
       <c r="A21" s="14" t="s">
         <v>15</v>
       </c>
@@ -1390,8 +1420,9 @@
       <c r="I21" s="19"/>
       <c r="J21" s="14"/>
       <c r="K21" s="19"/>
-    </row>
-    <row r="22" spans="1:11" ht="75">
+      <c r="L21" s="19"/>
+    </row>
+    <row r="22" spans="1:12" ht="75">
       <c r="A22" s="14" t="s">
         <v>15</v>
       </c>
@@ -1411,8 +1442,9 @@
       </c>
       <c r="J22" s="14"/>
       <c r="K22" s="19"/>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22" s="19"/>
+    </row>
+    <row r="23" spans="1:12">
       <c r="A23" s="14" t="s">
         <v>15</v>
       </c>
@@ -1430,6 +1462,7 @@
       <c r="I23" s="19"/>
       <c r="J23" s="14"/>
       <c r="K23" s="19"/>
+      <c r="L23" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Change the client visit form per partner's request #99
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_visit.xlsx
+++ b/config/itech-aurum/forms/app/client_visit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-81\itech-aurum\forms\app\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-99\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D2E6658-09D7-4BD3-A374-5B1617A1744B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CF4270-D0DA-4B8C-A7D5-61E219051A17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="153">
   <si>
     <t>type</t>
   </si>
@@ -366,6 +366,126 @@
   </si>
   <si>
     <t>instance::tag</t>
+  </si>
+  <si>
+    <t>select_one sites</t>
+  </si>
+  <si>
+    <t>site</t>
+  </si>
+  <si>
+    <t>Where did the man receive care?</t>
+  </si>
+  <si>
+    <t>select_one reviewers</t>
+  </si>
+  <si>
+    <t>reviewer</t>
+  </si>
+  <si>
+    <t>Who reviewed the client?</t>
+  </si>
+  <si>
+    <t>reviewers</t>
+  </si>
+  <si>
+    <t>DoH nurse</t>
+  </si>
+  <si>
+    <t>nurse</t>
+  </si>
+  <si>
+    <t>sites</t>
+  </si>
+  <si>
+    <t>district</t>
+  </si>
+  <si>
+    <t>districts</t>
+  </si>
+  <si>
+    <t>Ekurhuleni</t>
+  </si>
+  <si>
+    <t>Bojanala</t>
+  </si>
+  <si>
+    <t>ekurhuleni</t>
+  </si>
+  <si>
+    <t>bojanala</t>
+  </si>
+  <si>
+    <t>Tsakane Clinic</t>
+  </si>
+  <si>
+    <t>Katlehong Clinic</t>
+  </si>
+  <si>
+    <t>Mobile</t>
+  </si>
+  <si>
+    <t>Winnie Mandela Clinic</t>
+  </si>
+  <si>
+    <t>Bafokeng</t>
+  </si>
+  <si>
+    <t>Letlhabile</t>
+  </si>
+  <si>
+    <t>winnie_mandela</t>
+  </si>
+  <si>
+    <t>tsakane</t>
+  </si>
+  <si>
+    <t>katlehong</t>
+  </si>
+  <si>
+    <t>bafokeng</t>
+  </si>
+  <si>
+    <t>letlhabile</t>
+  </si>
+  <si>
+    <t>mogwase</t>
+  </si>
+  <si>
+    <t>mobile-e</t>
+  </si>
+  <si>
+    <t>mobile-b</t>
+  </si>
+  <si>
+    <t>Mogwase Clinic</t>
+  </si>
+  <si>
+    <t>select_one districts</t>
+  </si>
+  <si>
+    <t>${district} = district</t>
+  </si>
+  <si>
+    <t>not(${district} = '')</t>
+  </si>
+  <si>
+    <t>choice_filter</t>
+  </si>
+  <si>
+    <t>Dedicated/mobile VMMC team</t>
+  </si>
+  <si>
+    <t>team</t>
+  </si>
+  <si>
+    <t>location</t>
+  </si>
+  <si>
+    <t>District</t>
+  </si>
+  <si>
+    <t>Site</t>
   </si>
 </sst>
 </file>
@@ -930,16 +1050,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:M30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
+      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="22.375" style="7"/>
     <col min="2" max="2" width="21" style="7"/>
@@ -952,12 +1072,13 @@
     <col min="9" max="9" width="27.375" style="20" customWidth="1"/>
     <col min="10" max="10" width="12.5" style="7"/>
     <col min="11" max="11" width="20.625" style="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.875" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="1025" width="12.5" style="7"/>
-    <col min="1026" max="16384" width="9" style="7"/>
+    <col min="12" max="12" width="13.875" style="7" customWidth="1"/>
+    <col min="13" max="13" width="13.875" style="7" bestFit="1" customWidth="1"/>
+    <col min="14" max="1026" width="12.5" style="7"/>
+    <col min="1027" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="6" customFormat="1" ht="15.75">
+    <row r="1" spans="1:13" s="6" customFormat="1">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -992,10 +1113,13 @@
         <v>10</v>
       </c>
       <c r="L1" s="6" t="s">
+        <v>147</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:13" ht="15">
       <c r="A2" s="11" t="s">
         <v>11</v>
       </c>
@@ -1018,8 +1142,9 @@
       <c r="J2" s="11"/>
       <c r="K2" s="16"/>
       <c r="L2" s="16"/>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="16"/>
+    </row>
+    <row r="3" spans="1:13" ht="15">
       <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
@@ -1042,8 +1167,9 @@
       </c>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
-    </row>
-    <row r="4" spans="1:12">
+      <c r="M3" s="17"/>
+    </row>
+    <row r="4" spans="1:13" ht="15">
       <c r="A4" s="11" t="s">
         <v>15</v>
       </c>
@@ -1064,8 +1190,9 @@
       <c r="J4" s="10"/>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
-    </row>
-    <row r="5" spans="1:12">
+      <c r="M4" s="17"/>
+    </row>
+    <row r="5" spans="1:13" ht="15">
       <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
@@ -1084,8 +1211,9 @@
       <c r="J5" s="10"/>
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
-    </row>
-    <row r="6" spans="1:12">
+      <c r="M5" s="17"/>
+    </row>
+    <row r="6" spans="1:13" ht="15">
       <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
@@ -1110,8 +1238,9 @@
       <c r="J6" s="10"/>
       <c r="K6" s="17"/>
       <c r="L6" s="17"/>
-    </row>
-    <row r="7" spans="1:12">
+      <c r="M6" s="17"/>
+    </row>
+    <row r="7" spans="1:13" ht="15">
       <c r="A7" s="11" t="s">
         <v>18</v>
       </c>
@@ -1130,8 +1259,9 @@
       <c r="J7" s="10"/>
       <c r="K7" s="17"/>
       <c r="L7" s="17"/>
-    </row>
-    <row r="8" spans="1:12">
+      <c r="M7" s="17"/>
+    </row>
+    <row r="8" spans="1:13" ht="15">
       <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
@@ -1150,8 +1280,9 @@
       <c r="J8" s="10"/>
       <c r="K8" s="17"/>
       <c r="L8" s="17"/>
-    </row>
-    <row r="9" spans="1:12">
+      <c r="M8" s="17"/>
+    </row>
+    <row r="9" spans="1:13" ht="15">
       <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
@@ -1166,8 +1297,9 @@
       <c r="J9" s="10"/>
       <c r="K9" s="17"/>
       <c r="L9" s="17"/>
-    </row>
-    <row r="10" spans="1:12">
+      <c r="M9" s="17"/>
+    </row>
+    <row r="10" spans="1:13" ht="15">
       <c r="A10" s="11" t="s">
         <v>32</v>
       </c>
@@ -1182,11 +1314,13 @@
       <c r="J10" s="11"/>
       <c r="K10" s="16"/>
       <c r="L10" s="16"/>
-    </row>
-    <row r="11" spans="1:12">
+      <c r="M10" s="16"/>
+    </row>
+    <row r="11" spans="1:13" ht="15">
       <c r="L11" s="20"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" s="20"/>
+    </row>
+    <row r="12" spans="1:13" ht="15">
       <c r="A12" s="13" t="s">
         <v>33</v>
       </c>
@@ -1207,8 +1341,9 @@
         <v>35</v>
       </c>
       <c r="L12" s="18"/>
-    </row>
-    <row r="13" spans="1:12">
+      <c r="M12" s="18"/>
+    </row>
+    <row r="13" spans="1:13" ht="15">
       <c r="A13" s="13" t="s">
         <v>33</v>
       </c>
@@ -1229,8 +1364,9 @@
         <v>37</v>
       </c>
       <c r="L13" s="18"/>
-    </row>
-    <row r="14" spans="1:12">
+      <c r="M13" s="18"/>
+    </row>
+    <row r="14" spans="1:13" ht="15">
       <c r="A14" s="13" t="s">
         <v>33</v>
       </c>
@@ -1252,11 +1388,12 @@
       <c r="K14" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="L14" s="18" t="s">
+      <c r="L14" s="18"/>
+      <c r="M14" s="18" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:12" ht="105">
+    <row r="15" spans="1:13" ht="105">
       <c r="A15" s="14" t="s">
         <v>42</v>
       </c>
@@ -1275,8 +1412,9 @@
       <c r="J15" s="14"/>
       <c r="K15" s="19"/>
       <c r="L15" s="19"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="M15" s="19"/>
+    </row>
+    <row r="16" spans="1:13" ht="15">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -1297,8 +1435,9 @@
       <c r="J16" s="14"/>
       <c r="K16" s="19"/>
       <c r="L16" s="19"/>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="M16" s="19"/>
+    </row>
+    <row r="17" spans="1:13" ht="15">
       <c r="A17" s="14" t="s">
         <v>48</v>
       </c>
@@ -1321,8 +1460,9 @@
       <c r="J17" s="14"/>
       <c r="K17" s="19"/>
       <c r="L17" s="19"/>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="M17" s="19"/>
+    </row>
+    <row r="18" spans="1:13" ht="15">
       <c r="A18" s="14" t="s">
         <v>15</v>
       </c>
@@ -1345,124 +1485,273 @@
       <c r="J18" s="14"/>
       <c r="K18" s="19"/>
       <c r="L18" s="19"/>
-    </row>
-    <row r="19" spans="1:12" ht="25.5">
-      <c r="A19" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="C19" s="19" t="s">
-        <v>54</v>
-      </c>
+      <c r="M18" s="19"/>
+    </row>
+    <row r="19" spans="1:13" ht="15">
+      <c r="A19" s="14"/>
+      <c r="B19" s="14"/>
+      <c r="C19" s="19"/>
       <c r="D19" s="19"/>
       <c r="E19" s="14"/>
-      <c r="F19" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G19" s="21" t="s">
-        <v>55</v>
-      </c>
-      <c r="H19" s="21" t="s">
-        <v>106</v>
-      </c>
+      <c r="F19" s="14"/>
+      <c r="G19" s="21"/>
+      <c r="H19" s="19"/>
       <c r="I19" s="19"/>
-      <c r="J19" s="14" t="s">
-        <v>56</v>
-      </c>
+      <c r="J19" s="14"/>
       <c r="K19" s="19"/>
       <c r="L19" s="19"/>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="M19" s="19"/>
+    </row>
+    <row r="20" spans="1:13" ht="25.5">
       <c r="A20" s="14" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>107</v>
+        <v>54</v>
       </c>
       <c r="D20" s="19"/>
       <c r="E20" s="14"/>
       <c r="F20" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
+      <c r="G20" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="21" t="s">
+        <v>106</v>
+      </c>
       <c r="I20" s="19"/>
-      <c r="J20" s="14"/>
+      <c r="J20" s="14" t="s">
+        <v>56</v>
+      </c>
       <c r="K20" s="19"/>
       <c r="L20" s="19"/>
-    </row>
-    <row r="21" spans="1:12" ht="60">
+      <c r="M20" s="19"/>
+    </row>
+    <row r="21" spans="1:13" ht="15">
       <c r="A21" s="14" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>59</v>
+        <v>150</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>108</v>
-      </c>
-      <c r="D21" s="19" t="s">
-        <v>105</v>
-      </c>
-      <c r="E21" s="14"/>
+        <v>115</v>
+      </c>
+      <c r="D21" s="19"/>
+      <c r="E21" s="14" t="s">
+        <v>14</v>
+      </c>
       <c r="F21" s="14"/>
-      <c r="G21" s="21" t="s">
-        <v>111</v>
-      </c>
-      <c r="H21" s="21" t="s">
-        <v>109</v>
-      </c>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
       <c r="I21" s="19"/>
       <c r="J21" s="14"/>
       <c r="K21" s="19"/>
       <c r="L21" s="19"/>
-    </row>
-    <row r="22" spans="1:12" ht="75">
+      <c r="M21" s="19"/>
+    </row>
+    <row r="22" spans="1:13" ht="15">
       <c r="A22" s="14" t="s">
-        <v>15</v>
+        <v>144</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>60</v>
+        <v>123</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>110</v>
+        <v>151</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="14"/>
-      <c r="F22" s="14"/>
-      <c r="G22" s="19"/>
-      <c r="H22" s="19"/>
-      <c r="I22" s="19" t="s">
-        <v>61</v>
-      </c>
+      <c r="F22" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G22" s="21"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="19"/>
       <c r="J22" s="14"/>
       <c r="K22" s="19"/>
       <c r="L22" s="19"/>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="M22" s="19"/>
+    </row>
+    <row r="23" spans="1:13" ht="30">
       <c r="A23" s="14" t="s">
-        <v>15</v>
+        <v>113</v>
       </c>
       <c r="B23" s="14" t="s">
-        <v>62</v>
+        <v>114</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D23" s="19"/>
+        <v>152</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>146</v>
+      </c>
       <c r="E23" s="14"/>
-      <c r="F23" s="14"/>
-      <c r="G23" s="19"/>
-      <c r="H23" s="19"/>
+      <c r="F23" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G23" s="21"/>
+      <c r="H23" s="21"/>
       <c r="I23" s="19"/>
       <c r="J23" s="14"/>
       <c r="K23" s="19"/>
-      <c r="L23" s="19"/>
+      <c r="L23" s="19" t="s">
+        <v>145</v>
+      </c>
+      <c r="M23" s="19"/>
+    </row>
+    <row r="24" spans="1:13" ht="15">
+      <c r="A24" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24" s="14"/>
+      <c r="C24" s="19"/>
+      <c r="D24" s="19"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="19"/>
+      <c r="J24" s="14"/>
+      <c r="K24" s="19"/>
+      <c r="L24" s="19"/>
+      <c r="M24" s="19"/>
+    </row>
+    <row r="25" spans="1:13" ht="15">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="19"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="19"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="19"/>
+      <c r="L25" s="19"/>
+      <c r="M25" s="19"/>
+    </row>
+    <row r="26" spans="1:13" ht="15">
+      <c r="A26" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="B26" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="19"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="19"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="19"/>
+      <c r="L26" s="19"/>
+      <c r="M26" s="19"/>
+    </row>
+    <row r="27" spans="1:13" ht="15">
+      <c r="A27" s="14" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="14" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="19" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="19"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="19"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="19"/>
+      <c r="L27" s="19"/>
+      <c r="M27" s="19"/>
+    </row>
+    <row r="28" spans="1:13" ht="60">
+      <c r="A28" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="14" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>108</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>105</v>
+      </c>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="H28" s="21" t="s">
+        <v>109</v>
+      </c>
+      <c r="I28" s="19"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="19"/>
+      <c r="M28" s="19"/>
+    </row>
+    <row r="29" spans="1:13" ht="75">
+      <c r="A29" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>110</v>
+      </c>
+      <c r="D29" s="19"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="19"/>
+      <c r="H29" s="19"/>
+      <c r="I29" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="J29" s="14"/>
+      <c r="K29" s="19"/>
+      <c r="L29" s="19"/>
+      <c r="M29" s="19"/>
+    </row>
+    <row r="30" spans="1:13" ht="15">
+      <c r="A30" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="B30" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D30" s="19"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="19"/>
+      <c r="I30" s="19"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="19"/>
+      <c r="L30" s="19"/>
+      <c r="M30" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.74791666666666701" right="0.74791666666666701" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -1472,23 +1761,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="10" style="7"/>
-    <col min="2" max="2" width="12.5" style="7"/>
-    <col min="3" max="3" width="19.375" style="7"/>
+    <col min="2" max="2" width="15.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.5" style="7" bestFit="1" customWidth="1"/>
     <col min="4" max="1025" width="12.5" style="7"/>
     <col min="1026" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="6" customFormat="1" ht="15.75">
+    <row r="1" spans="1:4" s="6" customFormat="1" ht="15.75">
       <c r="A1" s="9" t="s">
         <v>64</v>
       </c>
@@ -1498,8 +1787,11 @@
       <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="8" t="s">
         <v>65</v>
       </c>
@@ -1510,7 +1802,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:4">
       <c r="A3" s="8" t="s">
         <v>65</v>
       </c>
@@ -1521,12 +1813,12 @@
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:4">
       <c r="A4" s="8"/>
       <c r="B4" s="8"/>
       <c r="C4" s="8"/>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:4">
       <c r="A5" s="8" t="s">
         <v>46</v>
       </c>
@@ -1537,7 +1829,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6" s="8" t="s">
         <v>46</v>
       </c>
@@ -1548,7 +1840,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:4">
       <c r="A7" s="8" t="s">
         <v>46</v>
       </c>
@@ -1559,7 +1851,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8" s="8" t="s">
         <v>46</v>
       </c>
@@ -1570,7 +1862,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:4">
       <c r="A9" s="8" t="s">
         <v>46</v>
       </c>
@@ -1581,7 +1873,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:4">
       <c r="A10" s="8" t="s">
         <v>46</v>
       </c>
@@ -1592,12 +1884,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:4">
       <c r="A11" s="8"/>
       <c r="B11" s="8"/>
       <c r="C11" s="8"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:4">
       <c r="A12" s="8" t="s">
         <v>58</v>
       </c>
@@ -1608,7 +1900,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:4">
       <c r="A13" s="8" t="s">
         <v>58</v>
       </c>
@@ -1619,7 +1911,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:4">
       <c r="A14" s="8" t="s">
         <v>58</v>
       </c>
@@ -1630,7 +1922,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:4">
       <c r="A15" s="8" t="s">
         <v>58</v>
       </c>
@@ -1639,6 +1931,162 @@
       </c>
       <c r="C15" s="8" t="s">
         <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>149</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>121</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>127</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="C25" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>139</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change request to remove some sites #99
</commit_message>
<xml_diff>
--- a/config/itech-aurum/forms/app/client_visit.xlsx
+++ b/config/itech-aurum/forms/app/client_visit.xlsx
@@ -1,24 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\work\medic\ssh-git\config-itech\config-itech-99\itech-aurum\forms\app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B5CF4270-D0DA-4B8C-A7D5-61E219051A17}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAABD308-509C-4371-BA5E-7975A5D583DA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
     <sheet name="choices" sheetId="2" r:id="rId2"/>
     <sheet name="settings" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
@@ -27,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="148">
   <si>
     <t>type</t>
   </si>
@@ -362,9 +371,6 @@
     <t>Name of Health Care Provider who reviewed the client</t>
   </si>
   <si>
-    <t>regex(., '^(AN|BL|IN|OT|PA|SD|SX|WD|OA)-[A-C]$')</t>
-  </si>
-  <si>
     <t>instance::tag</t>
   </si>
   <si>
@@ -416,15 +422,6 @@
     <t>bojanala</t>
   </si>
   <si>
-    <t>Tsakane Clinic</t>
-  </si>
-  <si>
-    <t>Katlehong Clinic</t>
-  </si>
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
     <t>Winnie Mandela Clinic</t>
   </si>
   <si>
@@ -437,12 +434,6 @@
     <t>winnie_mandela</t>
   </si>
   <si>
-    <t>tsakane</t>
-  </si>
-  <si>
-    <t>katlehong</t>
-  </si>
-  <si>
     <t>bafokeng</t>
   </si>
   <si>
@@ -452,12 +443,6 @@
     <t>mogwase</t>
   </si>
   <si>
-    <t>mobile-e</t>
-  </si>
-  <si>
-    <t>mobile-b</t>
-  </si>
-  <si>
     <t>Mogwase Clinic</t>
   </si>
   <si>
@@ -486,6 +471,15 @@
   </si>
   <si>
     <t>Site</t>
+  </si>
+  <si>
+    <t>bapong</t>
+  </si>
+  <si>
+    <t>Bapong Clinic</t>
+  </si>
+  <si>
+    <t>regex(., '^(AN|BL|IN|OT|PA|SD|SX|WD|OA)-[A-C]$') or regex(., '^(an|bl|in|ot|pa|sd|sx|wd|oa)-[a-c]$')</t>
   </si>
 </sst>
 </file>
@@ -1052,14 +1046,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C15" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="F23" sqref="F23"/>
+      <selection pane="bottomRight" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="22.375" style="7"/>
     <col min="2" max="2" width="21" style="7"/>
@@ -1078,7 +1072,7 @@
     <col min="1027" max="16384" width="9" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="6" customFormat="1">
+    <row r="1" spans="1:13" s="6" customFormat="1" ht="15.75">
       <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
@@ -1113,13 +1107,13 @@
         <v>10</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="15">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
       <c r="A2" s="11" t="s">
         <v>11</v>
       </c>
@@ -1144,7 +1138,7 @@
       <c r="L2" s="16"/>
       <c r="M2" s="16"/>
     </row>
-    <row r="3" spans="1:13" ht="15">
+    <row r="3" spans="1:13">
       <c r="A3" s="11" t="s">
         <v>15</v>
       </c>
@@ -1169,7 +1163,7 @@
       <c r="L3" s="17"/>
       <c r="M3" s="17"/>
     </row>
-    <row r="4" spans="1:13" ht="15">
+    <row r="4" spans="1:13">
       <c r="A4" s="11" t="s">
         <v>15</v>
       </c>
@@ -1192,7 +1186,7 @@
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
     </row>
-    <row r="5" spans="1:13" ht="15">
+    <row r="5" spans="1:13">
       <c r="A5" s="11" t="s">
         <v>11</v>
       </c>
@@ -1213,7 +1207,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
     </row>
-    <row r="6" spans="1:13" ht="15">
+    <row r="6" spans="1:13">
       <c r="A6" s="11" t="s">
         <v>24</v>
       </c>
@@ -1240,7 +1234,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
     </row>
-    <row r="7" spans="1:13" ht="15">
+    <row r="7" spans="1:13">
       <c r="A7" s="11" t="s">
         <v>18</v>
       </c>
@@ -1261,7 +1255,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
     </row>
-    <row r="8" spans="1:13" ht="15">
+    <row r="8" spans="1:13">
       <c r="A8" s="11" t="s">
         <v>18</v>
       </c>
@@ -1282,7 +1276,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
     </row>
-    <row r="9" spans="1:13" ht="15">
+    <row r="9" spans="1:13">
       <c r="A9" s="11" t="s">
         <v>32</v>
       </c>
@@ -1299,7 +1293,7 @@
       <c r="L9" s="17"/>
       <c r="M9" s="17"/>
     </row>
-    <row r="10" spans="1:13" ht="15">
+    <row r="10" spans="1:13">
       <c r="A10" s="11" t="s">
         <v>32</v>
       </c>
@@ -1316,11 +1310,11 @@
       <c r="L10" s="16"/>
       <c r="M10" s="16"/>
     </row>
-    <row r="11" spans="1:13" ht="15">
+    <row r="11" spans="1:13">
       <c r="L11" s="20"/>
       <c r="M11" s="20"/>
     </row>
-    <row r="12" spans="1:13" ht="15">
+    <row r="12" spans="1:13">
       <c r="A12" s="13" t="s">
         <v>33</v>
       </c>
@@ -1343,7 +1337,7 @@
       <c r="L12" s="18"/>
       <c r="M12" s="18"/>
     </row>
-    <row r="13" spans="1:13" ht="15">
+    <row r="13" spans="1:13">
       <c r="A13" s="13" t="s">
         <v>33</v>
       </c>
@@ -1366,7 +1360,7 @@
       <c r="L13" s="18"/>
       <c r="M13" s="18"/>
     </row>
-    <row r="14" spans="1:13" ht="15">
+    <row r="14" spans="1:13">
       <c r="A14" s="13" t="s">
         <v>33</v>
       </c>
@@ -1414,7 +1408,7 @@
       <c r="L15" s="19"/>
       <c r="M15" s="19"/>
     </row>
-    <row r="16" spans="1:13" ht="15">
+    <row r="16" spans="1:13">
       <c r="A16" s="14" t="s">
         <v>45</v>
       </c>
@@ -1437,7 +1431,7 @@
       <c r="L16" s="19"/>
       <c r="M16" s="19"/>
     </row>
-    <row r="17" spans="1:13" ht="15">
+    <row r="17" spans="1:13">
       <c r="A17" s="14" t="s">
         <v>48</v>
       </c>
@@ -1462,7 +1456,7 @@
       <c r="L17" s="19"/>
       <c r="M17" s="19"/>
     </row>
-    <row r="18" spans="1:13" ht="15">
+    <row r="18" spans="1:13">
       <c r="A18" s="14" t="s">
         <v>15</v>
       </c>
@@ -1487,7 +1481,7 @@
       <c r="L18" s="19"/>
       <c r="M18" s="19"/>
     </row>
-    <row r="19" spans="1:13" ht="15">
+    <row r="19" spans="1:13">
       <c r="A19" s="14"/>
       <c r="B19" s="14"/>
       <c r="C19" s="19"/>
@@ -1531,15 +1525,15 @@
       <c r="L20" s="19"/>
       <c r="M20" s="19"/>
     </row>
-    <row r="21" spans="1:13" ht="15">
+    <row r="21" spans="1:13">
       <c r="A21" s="14" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="14" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D21" s="19"/>
       <c r="E21" s="14" t="s">
@@ -1554,15 +1548,15 @@
       <c r="L21" s="19"/>
       <c r="M21" s="19"/>
     </row>
-    <row r="22" spans="1:13" ht="15">
+    <row r="22" spans="1:13">
       <c r="A22" s="14" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="B22" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="D22" s="19"/>
       <c r="E22" s="14"/>
@@ -1579,16 +1573,16 @@
     </row>
     <row r="23" spans="1:13" ht="30">
       <c r="A23" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="B23" s="14" t="s">
-        <v>114</v>
-      </c>
       <c r="C23" s="19" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D23" s="19" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="14" t="s">
@@ -1600,11 +1594,11 @@
       <c r="J23" s="14"/>
       <c r="K23" s="19"/>
       <c r="L23" s="19" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="M23" s="19"/>
     </row>
-    <row r="24" spans="1:13" ht="15">
+    <row r="24" spans="1:13">
       <c r="A24" s="14" t="s">
         <v>32</v>
       </c>
@@ -1621,7 +1615,7 @@
       <c r="L24" s="19"/>
       <c r="M24" s="19"/>
     </row>
-    <row r="25" spans="1:13" ht="15">
+    <row r="25" spans="1:13">
       <c r="A25" s="14"/>
       <c r="B25" s="14"/>
       <c r="C25" s="19"/>
@@ -1636,15 +1630,15 @@
       <c r="L25" s="19"/>
       <c r="M25" s="19"/>
     </row>
-    <row r="26" spans="1:13" ht="15">
+    <row r="26" spans="1:13">
       <c r="A26" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="B26" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="C26" s="19" t="s">
         <v>117</v>
-      </c>
-      <c r="C26" s="19" t="s">
-        <v>118</v>
       </c>
       <c r="D26" s="19"/>
       <c r="E26" s="14"/>
@@ -1659,7 +1653,7 @@
       <c r="L26" s="19"/>
       <c r="M26" s="19"/>
     </row>
-    <row r="27" spans="1:13" ht="15">
+    <row r="27" spans="1:13">
       <c r="A27" s="14" t="s">
         <v>57</v>
       </c>
@@ -1698,7 +1692,7 @@
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
       <c r="G28" s="21" t="s">
-        <v>111</v>
+        <v>147</v>
       </c>
       <c r="H28" s="21" t="s">
         <v>109</v>
@@ -1732,7 +1726,7 @@
       <c r="L29" s="19"/>
       <c r="M29" s="19"/>
     </row>
-    <row r="30" spans="1:13" ht="15">
+    <row r="30" spans="1:13">
       <c r="A30" s="14" t="s">
         <v>15</v>
       </c>
@@ -1761,11 +1755,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
+      <selection pane="bottomLeft" activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1788,7 +1782,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1935,68 +1929,68 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="7" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="C18" s="7" t="s">
         <v>119</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" s="7" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="7" t="s">
         <v>124</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C20" s="7" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C21" s="7" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>129</v>
@@ -2007,10 +2001,10 @@
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>130</v>
@@ -2021,13 +2015,13 @@
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C26" s="7" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>127</v>
@@ -2035,58 +2029,16 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="7" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>133</v>
+        <v>146</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
-      <c r="A28" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B28" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="C28" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="D28" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
-      <c r="A29" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B29" s="7" t="s">
-        <v>140</v>
-      </c>
-      <c r="C29" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="D29" s="7" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
-      <c r="A30" s="7" t="s">
-        <v>122</v>
-      </c>
-      <c r="B30" s="7" t="s">
-        <v>142</v>
-      </c>
-      <c r="C30" s="7" t="s">
-        <v>131</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>